<commit_message>
Update Metadata XLSX file
</commit_message>
<xml_diff>
--- a/data/xlsx/metadata.xlsx
+++ b/data/xlsx/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/sites/codeforiati/gov-id-finder-data/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F116A8-8E42-D44C-AEB1-78536367CA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8378644D-9E48-264C-90DE-2FECFD5791FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29820" yWindow="-2180" windowWidth="22260" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -165,9 +165,6 @@
   </si>
   <si>
     <t>https://www.mof.gov.kn/wp-content/uploads/2022/01/Volume-I-FOR-WEBSITE-1.pdf</t>
-  </si>
-  <si>
-    <t>https://mof.go.tz/docs/news/HESABU%202020.pdf</t>
   </si>
   <si>
     <t>Timor-leste</t>
@@ -514,6 +511,9 @@
   <si>
     <t>Zambia</t>
   </si>
+  <si>
+    <t>https://mof.go.tz/uploads/documents/en-1693215971-Vol%20II%20Recurrent%20Expenditure%20As%20Passed%202023.24.pdf</t>
+  </si>
 </sst>
 </file>
 
@@ -831,8 +831,8 @@
   </sheetPr>
   <dimension ref="A1:AA995"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -842,7 +842,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -879,7 +879,7 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -888,7 +888,7 @@
         <v>2020</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -916,7 +916,7 @@
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -953,16 +953,16 @@
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C4" s="1">
         <v>2019</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -990,7 +990,7 @@
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -1027,7 +1027,7 @@
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
@@ -1036,7 +1036,7 @@
         <v>2020</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1064,16 +1064,16 @@
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="1">
         <v>2019</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1101,10 +1101,10 @@
     </row>
     <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C8" s="1">
         <v>2014</v>
@@ -1138,10 +1138,10 @@
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C9" s="1">
         <v>2020</v>
@@ -1175,10 +1175,10 @@
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C10" s="1">
         <v>2020</v>
@@ -1212,10 +1212,10 @@
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C11" s="1">
         <v>2019</v>
@@ -1249,10 +1249,10 @@
     </row>
     <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C12" s="1">
         <v>2019</v>
@@ -1286,7 +1286,7 @@
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>11</v>
@@ -1323,10 +1323,10 @@
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C14" s="1">
         <v>2019</v>
@@ -1360,16 +1360,16 @@
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C15" s="1">
         <v>2022</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1397,10 +1397,10 @@
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C16" s="1">
         <v>2021</v>
@@ -1434,10 +1434,10 @@
     </row>
     <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C17" s="1">
         <v>2017</v>
@@ -1471,10 +1471,10 @@
     </row>
     <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C18" s="1">
         <v>2015</v>
@@ -1508,16 +1508,16 @@
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C19" s="1">
         <v>2020</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1545,16 +1545,16 @@
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C20">
         <v>2012</v>
       </c>
       <c r="D20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1582,16 +1582,16 @@
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C21" s="1">
         <v>2018</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -1619,10 +1619,10 @@
     </row>
     <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C22" s="1">
         <v>2019</v>
@@ -1656,16 +1656,16 @@
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C23" s="1">
         <v>2020</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -1693,10 +1693,10 @@
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C24" s="1">
         <v>2020</v>
@@ -1730,10 +1730,10 @@
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C25" s="1">
         <v>2021</v>
@@ -1767,16 +1767,16 @@
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C26">
         <v>2019</v>
       </c>
       <c r="D26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -1804,10 +1804,10 @@
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C27" s="1">
         <v>2020</v>
@@ -1841,10 +1841,10 @@
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C28" s="1">
         <v>2021</v>
@@ -1878,16 +1878,16 @@
     </row>
     <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C29" s="1">
         <v>2020</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1915,7 +1915,7 @@
     </row>
     <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>25</v>
@@ -1952,16 +1952,16 @@
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C31" s="1">
         <v>2017</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -1989,7 +1989,7 @@
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>27</v>
@@ -2026,10 +2026,10 @@
     </row>
     <row r="33" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C33" s="1">
         <v>2021</v>
@@ -2063,10 +2063,10 @@
     </row>
     <row r="34" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C34" s="1">
         <v>2020</v>
@@ -2100,10 +2100,10 @@
     </row>
     <row r="35" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C35" s="1">
         <v>2020</v>
@@ -2137,10 +2137,10 @@
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C36" s="1">
         <v>2019</v>
@@ -2174,10 +2174,10 @@
     </row>
     <row r="37" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C37" s="1">
         <v>2021</v>
@@ -2211,7 +2211,7 @@
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>30</v>
@@ -2248,10 +2248,10 @@
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C39" s="1">
         <v>2021</v>
@@ -2285,16 +2285,16 @@
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C40">
         <v>2022</v>
       </c>
       <c r="D40" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -2322,10 +2322,10 @@
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C41" s="1">
         <v>2019</v>
@@ -2359,10 +2359,10 @@
     </row>
     <row r="42" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C42" s="1">
         <v>2021</v>
@@ -2396,7 +2396,7 @@
     </row>
     <row r="43" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>40</v>
@@ -2433,16 +2433,16 @@
     </row>
     <row r="44" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C44" s="1">
         <v>2022</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -2470,7 +2470,7 @@
     </row>
     <row r="45" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>38</v>
@@ -2507,10 +2507,10 @@
     </row>
     <row r="46" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C46" s="1">
         <v>2020</v>
@@ -2544,16 +2544,16 @@
     </row>
     <row r="47" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C47">
         <v>2019</v>
       </c>
       <c r="D47" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -2581,16 +2581,16 @@
     </row>
     <row r="48" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C48" s="1">
         <v>2020</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -2618,16 +2618,16 @@
     </row>
     <row r="49" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C49" s="1">
         <v>2018</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -2653,18 +2653,18 @@
       <c r="Z49" s="1"/>
       <c r="AA49" s="1"/>
     </row>
-    <row r="50" spans="1:27" ht="14" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C50" s="1">
         <v>2020</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>44</v>
+      <c r="D50" s="5" t="s">
+        <v>159</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -2692,16 +2692,16 @@
     </row>
     <row r="51" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C51" s="1">
         <v>2020</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -2729,16 +2729,16 @@
     </row>
     <row r="52" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C52" s="1">
         <v>2018</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -2766,16 +2766,16 @@
     </row>
     <row r="53" spans="1:27" ht="56" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C53" s="1">
         <v>2021</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>

</xml_diff>

<commit_message>
Update source of Tanzania data
</commit_message>
<xml_diff>
--- a/data/xlsx/metadata.xlsx
+++ b/data/xlsx/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/sites/codeforiati/gov-id-finder-data/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8378644D-9E48-264C-90DE-2FECFD5791FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192E782E-0080-CC4C-86A4-CADAA711861B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29820" yWindow="-2180" windowWidth="22260" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="161">
   <si>
     <t>Country_name</t>
   </si>
@@ -514,6 +514,9 @@
   <si>
     <t>https://mof.go.tz/uploads/documents/en-1693215971-Vol%20II%20Recurrent%20Expenditure%20As%20Passed%202023.24.pdf</t>
   </si>
+  <si>
+    <t>2023/2024</t>
+  </si>
 </sst>
 </file>
 
@@ -831,13 +834,13 @@
   </sheetPr>
   <dimension ref="A1:AA995"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="43.6640625" customWidth="1"/>
+    <col min="4" max="4" width="74.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2653,15 +2656,15 @@
       <c r="Z49" s="1"/>
       <c r="AA49" s="1"/>
     </row>
-    <row r="50" spans="1:27" ht="42" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>98</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C50" s="1">
-        <v>2020</v>
+      <c r="C50" s="1" t="s">
+        <v>160</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>159</v>

</xml_diff>

<commit_message>
Add Congo and Namibia
</commit_message>
<xml_diff>
--- a/data/xlsx/metadata.xlsx
+++ b/data/xlsx/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/sites/codeforiati/gov-id-finder-data/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64BDA676-5C1D-9147-B37D-0ACEA13C1168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA2BE8C-23CD-C24E-82FF-9DB10796E468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41740" yWindow="-2180" windowWidth="22260" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41740" yWindow="-2200" windowWidth="22260" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="183">
   <si>
     <t>Country_name</t>
   </si>
@@ -565,6 +565,24 @@
   <si>
     <t>https://www.treasury.gov.za/documents/national%20budget/2024/excelFormat.aspx</t>
   </si>
+  <si>
+    <t>CG</t>
+  </si>
+  <si>
+    <t>Republic of the Congo</t>
+  </si>
+  <si>
+    <t>https://www.sgg.cg/JO/2023/congo-jo-2023-04-sp.pdf</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>https://mfpe.gov.na/budget/-/document_library/dcey/view_file/3365197</t>
+  </si>
 </sst>
 </file>
 
@@ -643,7 +661,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -654,14 +672,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -881,10 +908,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AA1000"/>
+  <dimension ref="A1:AA1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -893,7 +920,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -933,13 +960,13 @@
       <c r="A2" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1">
         <v>2020</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>121</v>
       </c>
       <c r="E2" s="1"/>
@@ -970,7 +997,7 @@
       <c r="A3" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1">
@@ -1007,7 +1034,7 @@
       <c r="A4" t="s">
         <v>106</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="8" t="s">
         <v>126</v>
       </c>
       <c r="C4" s="1">
@@ -1044,7 +1071,7 @@
       <c r="A5" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1">
@@ -1081,13 +1108,13 @@
       <c r="A6" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1">
         <v>2020</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>122</v>
       </c>
       <c r="E6" s="1"/>
@@ -1118,13 +1145,13 @@
       <c r="A7" t="s">
         <v>112</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="8" t="s">
         <v>58</v>
       </c>
       <c r="C7" s="1">
         <v>2019</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>59</v>
       </c>
       <c r="E7" s="1"/>
@@ -1155,7 +1182,7 @@
       <c r="A8" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="8" t="s">
         <v>127</v>
       </c>
       <c r="C8" s="1">
@@ -1192,7 +1219,7 @@
       <c r="A9" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="8" t="s">
         <v>128</v>
       </c>
       <c r="C9" s="1">
@@ -1229,13 +1256,13 @@
       <c r="A10" t="s">
         <v>161</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="9" t="s">
         <v>162</v>
       </c>
       <c r="C10" t="s">
         <v>160</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>163</v>
       </c>
       <c r="E10" s="1"/>
@@ -1266,7 +1293,7 @@
       <c r="A11" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="8" t="s">
         <v>129</v>
       </c>
       <c r="C11" s="1">
@@ -1303,7 +1330,7 @@
       <c r="A12" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="8" t="s">
         <v>130</v>
       </c>
       <c r="C12" s="1">
@@ -1337,17 +1364,17 @@
       <c r="AA12" s="1"/>
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
-        <v>69</v>
+      <c r="A13" s="5" t="s">
+        <v>177</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>131</v>
+      <c r="B13" s="8" t="s">
+        <v>178</v>
       </c>
       <c r="C13" s="1">
-        <v>2019</v>
+        <v>2024</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>14</v>
+      <c r="D13" s="4" t="s">
+        <v>179</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1375,16 +1402,16 @@
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>11</v>
+      <c r="B14" s="8" t="s">
+        <v>131</v>
       </c>
       <c r="C14" s="1">
         <v>2019</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1412,16 +1439,16 @@
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>132</v>
+      <c r="B15" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="C15" s="1">
         <v>2019</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1449,16 +1476,16 @@
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>133</v>
+      <c r="B16" s="8" t="s">
+        <v>132</v>
       </c>
       <c r="C16" s="1">
-        <v>2022</v>
+        <v>2019</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1486,16 +1513,16 @@
     </row>
     <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>134</v>
+      <c r="B17" s="8" t="s">
+        <v>133</v>
       </c>
       <c r="C17" s="1">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1523,16 +1550,16 @@
     </row>
     <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>135</v>
+      <c r="B18" s="8" t="s">
+        <v>134</v>
       </c>
       <c r="C18" s="1">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -1560,16 +1587,16 @@
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>136</v>
+      <c r="B19" s="8" t="s">
+        <v>135</v>
       </c>
       <c r="C19" s="1">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1597,16 +1624,16 @@
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>137</v>
+      <c r="B20" s="8" t="s">
+        <v>136</v>
       </c>
       <c r="C20" s="1">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1634,16 +1661,16 @@
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>115</v>
+      <c r="B21" s="8" t="s">
+        <v>137</v>
       </c>
-      <c r="C21">
-        <v>2012</v>
+      <c r="C21" s="1">
+        <v>2020</v>
       </c>
-      <c r="D21" t="s">
-        <v>116</v>
+      <c r="D21" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -1671,16 +1698,16 @@
     </row>
     <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>138</v>
+      <c r="B22" s="10" t="s">
+        <v>115</v>
       </c>
-      <c r="C22" s="1">
-        <v>2018</v>
+      <c r="C22">
+        <v>2012</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>54</v>
+      <c r="D22" t="s">
+        <v>116</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1708,16 +1735,16 @@
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>139</v>
+      <c r="B23" s="8" t="s">
+        <v>138</v>
       </c>
       <c r="C23" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -1745,16 +1772,16 @@
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>140</v>
+      <c r="B24" s="8" t="s">
+        <v>139</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>164</v>
+      <c r="C24" s="1">
+        <v>2019</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>123</v>
+      <c r="D24" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1782,16 +1809,16 @@
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>141</v>
+      <c r="B25" s="8" t="s">
+        <v>140</v>
       </c>
-      <c r="C25" s="1">
-        <v>2020</v>
+      <c r="C25" s="1" t="s">
+        <v>164</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>21</v>
+      <c r="D25" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -1819,16 +1846,16 @@
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>142</v>
+      <c r="B26" s="8" t="s">
+        <v>141</v>
       </c>
       <c r="C26" s="1">
-        <v>2021</v>
+        <v>2020</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>43</v>
+      <c r="D26" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -1856,16 +1883,16 @@
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>117</v>
+      <c r="B27" s="8" t="s">
+        <v>142</v>
       </c>
-      <c r="C27">
-        <v>2019</v>
+      <c r="C27" s="1">
+        <v>2021</v>
       </c>
-      <c r="D27" t="s">
-        <v>118</v>
+      <c r="D27" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -1893,16 +1920,16 @@
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>143</v>
+      <c r="B28" s="10" t="s">
+        <v>117</v>
       </c>
-      <c r="C28" s="1">
-        <v>2020</v>
+      <c r="C28">
+        <v>2019</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>23</v>
+      <c r="D28" t="s">
+        <v>118</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -1930,16 +1957,16 @@
     </row>
     <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>144</v>
+      <c r="B29" s="8" t="s">
+        <v>143</v>
       </c>
       <c r="C29" s="1">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1966,17 +1993,17 @@
       <c r="AA29" s="1"/>
     </row>
     <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="6" t="s">
-        <v>165</v>
+      <c r="A30" t="s">
+        <v>78</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>166</v>
+      <c r="B30" s="8" t="s">
+        <v>144</v>
       </c>
       <c r="C30" s="1">
         <v>2021</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>167</v>
+      <c r="D30" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -2003,17 +2030,17 @@
       <c r="AA30" s="1"/>
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" t="s">
-        <v>80</v>
+      <c r="A31" s="5" t="s">
+        <v>165</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>145</v>
+      <c r="B31" s="8" t="s">
+        <v>166</v>
       </c>
       <c r="C31" s="1">
-        <v>2020</v>
+        <v>2021</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>124</v>
+      <c r="D31" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -2041,16 +2068,16 @@
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>25</v>
+      <c r="B32" s="8" t="s">
+        <v>145</v>
       </c>
       <c r="C32" s="1">
         <v>2020</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>26</v>
+      <c r="D32" s="4" t="s">
+        <v>124</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2078,16 +2105,16 @@
     </row>
     <row r="33" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>146</v>
+      <c r="B33" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="C33" s="1">
-        <v>2017</v>
+        <v>2020</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>125</v>
+      <c r="D33" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -2115,16 +2142,16 @@
     </row>
     <row r="34" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>27</v>
+      <c r="B34" s="8" t="s">
+        <v>146</v>
       </c>
       <c r="C34" s="1">
-        <v>2020</v>
+        <v>2017</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>28</v>
+      <c r="D34" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -2152,16 +2179,16 @@
     </row>
     <row r="35" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>147</v>
+      <c r="B35" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="C35" s="1">
-        <v>2021</v>
+        <v>2020</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>24</v>
+      <c r="D35" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -2189,16 +2216,16 @@
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>148</v>
+      <c r="B36" s="8" t="s">
+        <v>147</v>
       </c>
       <c r="C36" s="1">
-        <v>2020</v>
+        <v>2021</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>29</v>
+      <c r="D36" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -2226,16 +2253,16 @@
     </row>
     <row r="37" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>149</v>
+      <c r="B37" s="8" t="s">
+        <v>148</v>
       </c>
       <c r="C37" s="1">
         <v>2020</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -2262,17 +2289,17 @@
       <c r="AA37" s="1"/>
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="6" t="s">
-        <v>168</v>
+      <c r="A38" s="5" t="s">
+        <v>180</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>169</v>
+      <c r="B38" s="8" t="s">
+        <v>181</v>
       </c>
       <c r="C38" s="1">
         <v>2024</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>170</v>
+      <c r="D38" s="4" t="s">
+        <v>182</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2300,16 +2327,16 @@
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>150</v>
+      <c r="B39" s="8" t="s">
+        <v>149</v>
       </c>
       <c r="C39" s="1">
-        <v>2019</v>
+        <v>2020</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>33</v>
+      <c r="D39" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -2336,17 +2363,17 @@
       <c r="AA39" s="1"/>
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" t="s">
-        <v>87</v>
+      <c r="A40" s="5" t="s">
+        <v>168</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>151</v>
+      <c r="B40" s="8" t="s">
+        <v>169</v>
       </c>
       <c r="C40" s="1">
-        <v>2021</v>
+        <v>2024</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>32</v>
+      <c r="D40" s="4" t="s">
+        <v>170</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -2374,16 +2401,16 @@
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>30</v>
+      <c r="B41" s="8" t="s">
+        <v>150</v>
       </c>
       <c r="C41" s="1">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -2411,16 +2438,16 @@
     </row>
     <row r="42" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>152</v>
+      <c r="B42" s="8" t="s">
+        <v>151</v>
       </c>
       <c r="C42" s="1">
         <v>2021</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -2447,17 +2474,17 @@
       <c r="AA42" s="1"/>
     </row>
     <row r="43" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="6" t="s">
-        <v>92</v>
+      <c r="A43" t="s">
+        <v>86</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>119</v>
+      <c r="B43" s="7" t="s">
+        <v>30</v>
       </c>
-      <c r="C43">
-        <v>2022</v>
+      <c r="C43" s="1">
+        <v>2021</v>
       </c>
-      <c r="D43" t="s">
-        <v>120</v>
+      <c r="D43" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -2485,16 +2512,16 @@
     </row>
     <row r="44" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>153</v>
+      <c r="B44" s="8" t="s">
+        <v>152</v>
       </c>
       <c r="C44" s="1">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -2521,17 +2548,17 @@
       <c r="AA44" s="1"/>
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" t="s">
-        <v>93</v>
+      <c r="A45" s="5" t="s">
+        <v>92</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>154</v>
+      <c r="B45" s="10" t="s">
+        <v>119</v>
       </c>
-      <c r="C45" s="1">
-        <v>2021</v>
+      <c r="C45">
+        <v>2022</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>37</v>
+      <c r="D45" t="s">
+        <v>120</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -2559,16 +2586,16 @@
     </row>
     <row r="46" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>40</v>
+      <c r="B46" s="8" t="s">
+        <v>153</v>
       </c>
       <c r="C46" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -2596,16 +2623,16 @@
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>155</v>
+      <c r="B47" s="8" t="s">
+        <v>154</v>
       </c>
       <c r="C47" s="1">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -2631,18 +2658,18 @@
       <c r="Z47" s="1"/>
       <c r="AA47" s="1"/>
     </row>
-    <row r="48" spans="1:27" ht="14" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>38</v>
+      <c r="B48" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="C48" s="1">
         <v>2020</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -2668,18 +2695,18 @@
       <c r="Z48" s="1"/>
       <c r="AA48" s="1"/>
     </row>
-    <row r="49" spans="1:27" ht="28" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>156</v>
+      <c r="B49" s="8" t="s">
+        <v>155</v>
       </c>
       <c r="C49" s="1">
-        <v>2020</v>
+        <v>2022</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -2706,17 +2733,17 @@
       <c r="AA49" s="1"/>
     </row>
     <row r="50" spans="1:27" ht="14" x14ac:dyDescent="0.15">
-      <c r="A50" s="6" t="s">
-        <v>171</v>
+      <c r="A50" t="s">
+        <v>94</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>172</v>
+      <c r="B50" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="C50" s="1">
-        <v>2024</v>
+        <v>2020</v>
       </c>
-      <c r="D50" s="5" t="s">
-        <v>173</v>
+      <c r="D50" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -2742,18 +2769,18 @@
       <c r="Z50" s="1"/>
       <c r="AA50" s="1"/>
     </row>
-    <row r="51" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
-      <c r="B51" s="6" t="s">
-        <v>113</v>
+      <c r="B51" s="8" t="s">
+        <v>156</v>
       </c>
-      <c r="C51">
-        <v>2019</v>
+      <c r="C51" s="1">
+        <v>2020</v>
       </c>
-      <c r="D51" t="s">
-        <v>114</v>
+      <c r="D51" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -2780,17 +2807,17 @@
       <c r="AA51" s="1"/>
     </row>
     <row r="52" spans="1:27" ht="14" x14ac:dyDescent="0.15">
-      <c r="A52" t="s">
-        <v>100</v>
+      <c r="A52" s="5" t="s">
+        <v>171</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>46</v>
+      <c r="B52" s="8" t="s">
+        <v>172</v>
       </c>
       <c r="C52" s="1">
-        <v>2020</v>
+        <v>2024</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>47</v>
+      <c r="D52" s="4" t="s">
+        <v>173</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -2816,18 +2843,18 @@
       <c r="Z52" s="1"/>
       <c r="AA52" s="1"/>
     </row>
-    <row r="53" spans="1:27" ht="14" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>44</v>
+      <c r="B53" s="10" t="s">
+        <v>113</v>
       </c>
-      <c r="C53" s="1">
-        <v>2018</v>
+      <c r="C53">
+        <v>2019</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>45</v>
+      <c r="D53" t="s">
+        <v>114</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -2853,18 +2880,18 @@
       <c r="Z53" s="1"/>
       <c r="AA53" s="1"/>
     </row>
-    <row r="54" spans="1:27" ht="28" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>157</v>
+      <c r="B54" s="8" t="s">
+        <v>46</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>160</v>
+      <c r="C54" s="1">
+        <v>2020</v>
       </c>
-      <c r="D54" s="5" t="s">
-        <v>159</v>
+      <c r="D54" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -2892,16 +2919,16 @@
     </row>
     <row r="55" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>48</v>
+      <c r="B55" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="C55" s="1">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -2927,18 +2954,18 @@
       <c r="Z55" s="1"/>
       <c r="AA55" s="1"/>
     </row>
-    <row r="56" spans="1:27" ht="14" x14ac:dyDescent="0.15">
-      <c r="A56" s="6" t="s">
-        <v>174</v>
+    <row r="56" spans="1:27" ht="28" x14ac:dyDescent="0.15">
+      <c r="A56" t="s">
+        <v>98</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>175</v>
+      <c r="B56" s="8" t="s">
+        <v>157</v>
       </c>
-      <c r="C56" s="1">
-        <v>2024</v>
+      <c r="C56" s="1" t="s">
+        <v>160</v>
       </c>
-      <c r="D56" s="5" t="s">
-        <v>176</v>
+      <c r="D56" s="4" t="s">
+        <v>159</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
@@ -2966,16 +2993,16 @@
     </row>
     <row r="57" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>158</v>
+      <c r="B57" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="C57" s="1">
-        <v>2018</v>
+        <v>2020</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>50</v>
+      <c r="D57" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -3001,18 +3028,18 @@
       <c r="Z57" s="1"/>
       <c r="AA57" s="1"/>
     </row>
-    <row r="58" spans="1:27" ht="42" x14ac:dyDescent="0.15">
-      <c r="A58" t="s">
-        <v>103</v>
+    <row r="58" spans="1:27" ht="14" x14ac:dyDescent="0.15">
+      <c r="A58" s="5" t="s">
+        <v>174</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>51</v>
+      <c r="B58" s="8" t="s">
+        <v>175</v>
       </c>
       <c r="C58" s="1">
-        <v>2021</v>
+        <v>2024</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>52</v>
+      <c r="D58" s="4" t="s">
+        <v>176</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -3038,10 +3065,19 @@
       <c r="Z58" s="1"/>
       <c r="AA58" s="1"/>
     </row>
-    <row r="59" spans="1:27" ht="13" x14ac:dyDescent="0.15">
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
+    <row r="59" spans="1:27" ht="14" x14ac:dyDescent="0.15">
+      <c r="A59" t="s">
+        <v>102</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C59" s="1">
+        <v>2018</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -3066,10 +3102,19 @@
       <c r="Z59" s="1"/>
       <c r="AA59" s="1"/>
     </row>
-    <row r="60" spans="1:27" ht="13" x14ac:dyDescent="0.15">
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
+    <row r="60" spans="1:27" ht="42" x14ac:dyDescent="0.15">
+      <c r="A60" t="s">
+        <v>103</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C60" s="1">
+        <v>2021</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -29414,9 +29459,65 @@
       <c r="Z1000" s="1"/>
       <c r="AA1000" s="1"/>
     </row>
+    <row r="1001" spans="2:27" ht="13" x14ac:dyDescent="0.15">
+      <c r="B1001" s="1"/>
+      <c r="C1001" s="1"/>
+      <c r="D1001" s="1"/>
+      <c r="E1001" s="1"/>
+      <c r="F1001" s="1"/>
+      <c r="G1001" s="1"/>
+      <c r="H1001" s="1"/>
+      <c r="I1001" s="1"/>
+      <c r="J1001" s="1"/>
+      <c r="K1001" s="1"/>
+      <c r="L1001" s="1"/>
+      <c r="M1001" s="1"/>
+      <c r="N1001" s="1"/>
+      <c r="O1001" s="1"/>
+      <c r="P1001" s="1"/>
+      <c r="Q1001" s="1"/>
+      <c r="R1001" s="1"/>
+      <c r="S1001" s="1"/>
+      <c r="T1001" s="1"/>
+      <c r="U1001" s="1"/>
+      <c r="V1001" s="1"/>
+      <c r="W1001" s="1"/>
+      <c r="X1001" s="1"/>
+      <c r="Y1001" s="1"/>
+      <c r="Z1001" s="1"/>
+      <c r="AA1001" s="1"/>
+    </row>
+    <row r="1002" spans="2:27" ht="13" x14ac:dyDescent="0.15">
+      <c r="B1002" s="1"/>
+      <c r="C1002" s="1"/>
+      <c r="D1002" s="1"/>
+      <c r="E1002" s="1"/>
+      <c r="F1002" s="1"/>
+      <c r="G1002" s="1"/>
+      <c r="H1002" s="1"/>
+      <c r="I1002" s="1"/>
+      <c r="J1002" s="1"/>
+      <c r="K1002" s="1"/>
+      <c r="L1002" s="1"/>
+      <c r="M1002" s="1"/>
+      <c r="N1002" s="1"/>
+      <c r="O1002" s="1"/>
+      <c r="P1002" s="1"/>
+      <c r="Q1002" s="1"/>
+      <c r="R1002" s="1"/>
+      <c r="S1002" s="1"/>
+      <c r="T1002" s="1"/>
+      <c r="U1002" s="1"/>
+      <c r="V1002" s="1"/>
+      <c r="W1002" s="1"/>
+      <c r="X1002" s="1"/>
+      <c r="Y1002" s="1"/>
+      <c r="Z1002" s="1"/>
+      <c r="AA1002" s="1"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D58">
-    <sortCondition ref="A53:A58"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D60">
+    <sortCondition ref="A55:A60"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -29425,53 +29526,55 @@
     <hyperlink ref="D8" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="D5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="D6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="D14" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D15" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="D12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="D13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D14" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="D11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="D15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="D17" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="D18" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="D19" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D23" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="D24" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="D25" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="D29" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="D28" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="D31" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="D35" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="D32" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="D34" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="D36" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="D33" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="D41" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="D40" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="D39" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="D37" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="D44" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="D42" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="D45" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="D48" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="D46" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="D49" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="D26" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="D54" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="D53" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="D52" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="D55" r:id="rId40" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="D57" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="D58" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="D16" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="D22" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="D16" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D18" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D19" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D20" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D24" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D25" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D26" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="D30" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="D29" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="D32" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="D36" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="D33" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="D35" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="D37" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="D34" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D43" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="D42" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="D41" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="D39" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="D46" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="D44" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="D47" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="D50" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="D48" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="D51" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="D27" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="D56" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="D55" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="D54" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="D57" r:id="rId40" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="D59" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="D60" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="D17" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="D23" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
     <hyperlink ref="D4" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="D47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="D20" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="D49" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="D21" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
     <hyperlink ref="D7" r:id="rId48" xr:uid="{AEC54F8E-3B97-0D42-BDBF-81F51CF558FA}"/>
     <hyperlink ref="D10" r:id="rId49" xr:uid="{531FF59E-3ED0-7647-A071-9938F307CC65}"/>
-    <hyperlink ref="D30" r:id="rId50" xr:uid="{F44184D1-3BA6-CA4D-B592-38E9B7DD9585}"/>
-    <hyperlink ref="D38" r:id="rId51" xr:uid="{9B0CA447-45E8-D346-B56C-D40A5B7E7394}"/>
-    <hyperlink ref="D50" r:id="rId52" xr:uid="{6BBC2247-F5A6-2B4C-BCC0-65AE168D0F4C}"/>
-    <hyperlink ref="D56" r:id="rId53" xr:uid="{08F79F8D-E59F-AA49-A346-A986D8DD0952}"/>
+    <hyperlink ref="D31" r:id="rId50" xr:uid="{F44184D1-3BA6-CA4D-B592-38E9B7DD9585}"/>
+    <hyperlink ref="D40" r:id="rId51" xr:uid="{9B0CA447-45E8-D346-B56C-D40A5B7E7394}"/>
+    <hyperlink ref="D52" r:id="rId52" xr:uid="{6BBC2247-F5A6-2B4C-BCC0-65AE168D0F4C}"/>
+    <hyperlink ref="D58" r:id="rId53" xr:uid="{08F79F8D-E59F-AA49-A346-A986D8DD0952}"/>
+    <hyperlink ref="D13" r:id="rId54" xr:uid="{7C13DFA2-9F0D-4A4B-8033-EEC7EC90A886}"/>
+    <hyperlink ref="D38" r:id="rId55" xr:uid="{DC9C8D1E-F476-4A4E-902C-35F1A9CEBD2C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Mali to 2024 and remove duplicates
</commit_message>
<xml_diff>
--- a/data/xlsx/metadata.xlsx
+++ b/data/xlsx/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/sites/codeforiati/gov-id-finder-data/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B3CD79-A66B-5048-A6D0-EF3149B60AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD53396-CBA1-074E-AD31-513A8C478490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="41740" yWindow="-2200" windowWidth="22260" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,9 +111,6 @@
   </si>
   <si>
     <t>Mali</t>
-  </si>
-  <si>
-    <t>https://datacatalog.worldbank.org/search/dataset/0042337</t>
   </si>
   <si>
     <t>Mauritania</t>
@@ -592,6 +589,9 @@
   <si>
     <t>https://mofep.gov.gh/sites/default/files/budget-statements/2023-Appropriation-Act.pdf</t>
   </si>
+  <si>
+    <t>https://finances.ml/node/608</t>
+  </si>
 </sst>
 </file>
 
@@ -920,7 +920,7 @@
   <dimension ref="A1:AA1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -930,7 +930,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -967,7 +967,7 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>3</v>
@@ -976,7 +976,7 @@
         <v>2020</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1004,7 +1004,7 @@
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>4</v>
@@ -1041,16 +1041,16 @@
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C4" s="1">
         <v>2019</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -1078,7 +1078,7 @@
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>8</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>10</v>
@@ -1124,7 +1124,7 @@
         <v>2020</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1152,16 +1152,16 @@
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="1">
         <v>2019</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1189,10 +1189,10 @@
     </row>
     <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C8" s="1">
         <v>2014</v>
@@ -1226,10 +1226,10 @@
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C9" s="1">
         <v>2020</v>
@@ -1263,16 +1263,16 @@
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
+        <v>159</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>161</v>
-      </c>
       <c r="C10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1300,10 +1300,10 @@
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C11" s="1">
         <v>2020</v>
@@ -1337,10 +1337,10 @@
     </row>
     <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C12" s="1">
         <v>2019</v>
@@ -1374,16 +1374,16 @@
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C13" s="1">
         <v>2024</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1411,10 +1411,10 @@
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C14" s="1">
         <v>2019</v>
@@ -1448,7 +1448,7 @@
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>11</v>
@@ -1485,10 +1485,10 @@
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C16" s="1">
         <v>2019</v>
@@ -1522,16 +1522,16 @@
     </row>
     <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C17" s="1">
         <v>2023</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1559,10 +1559,10 @@
     </row>
     <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C18" s="1">
         <v>2021</v>
@@ -1596,10 +1596,10 @@
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C19" s="1">
         <v>2017</v>
@@ -1633,16 +1633,16 @@
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C20" s="1">
         <v>2022</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1670,10 +1670,10 @@
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C21" s="1">
         <v>2015</v>
@@ -1707,16 +1707,16 @@
     </row>
     <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C22" s="1">
         <v>2020</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1744,16 +1744,16 @@
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C23">
         <v>2012</v>
       </c>
       <c r="D23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -1781,16 +1781,16 @@
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C24" s="1">
         <v>2018</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1818,10 +1818,10 @@
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C25" s="1">
         <v>2019</v>
@@ -1855,16 +1855,16 @@
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -1892,10 +1892,10 @@
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C27" s="1">
         <v>2020</v>
@@ -1929,16 +1929,16 @@
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C28" s="1">
         <v>2021</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -1966,16 +1966,16 @@
     </row>
     <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C29">
         <v>2019</v>
       </c>
       <c r="D29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -2003,10 +2003,10 @@
     </row>
     <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C30" s="1">
         <v>2020</v>
@@ -2040,10 +2040,10 @@
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C31" s="1">
         <v>2021</v>
@@ -2077,16 +2077,16 @@
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C32" s="1">
         <v>2021</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2114,16 +2114,16 @@
     </row>
     <row r="33" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C33" s="1">
         <v>2020</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -2151,16 +2151,16 @@
     </row>
     <row r="34" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C34" s="1">
-        <v>2020</v>
+        <v>2024</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>26</v>
+        <v>185</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -2188,16 +2188,16 @@
     </row>
     <row r="35" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C35" s="1">
         <v>2017</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -2225,16 +2225,16 @@
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C36" s="1">
         <v>2020</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -2262,10 +2262,10 @@
     </row>
     <row r="37" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C37" s="1">
         <v>2021</v>
@@ -2299,16 +2299,16 @@
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C38" s="1">
         <v>2020</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2336,16 +2336,16 @@
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C39" s="1">
         <v>2024</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -2373,16 +2373,16 @@
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C40" s="1">
         <v>2020</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -2410,16 +2410,16 @@
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C41" s="1">
         <v>2024</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -2447,16 +2447,16 @@
     </row>
     <row r="42" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C42" s="1">
         <v>2019</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -2484,16 +2484,16 @@
     </row>
     <row r="43" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C43" s="1">
         <v>2021</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -2521,16 +2521,16 @@
     </row>
     <row r="44" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C44" s="1">
         <v>2021</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -2558,16 +2558,16 @@
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C45" s="1">
         <v>2021</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -2595,16 +2595,16 @@
     </row>
     <row r="46" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C46">
         <v>2022</v>
       </c>
       <c r="D46" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -2632,16 +2632,16 @@
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C47" s="1">
         <v>2019</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -2669,16 +2669,16 @@
     </row>
     <row r="48" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C48" s="1">
         <v>2021</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -2706,16 +2706,16 @@
     </row>
     <row r="49" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C49" s="1">
         <v>2020</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -2743,16 +2743,16 @@
     </row>
     <row r="50" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C50" s="1">
         <v>2022</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -2780,16 +2780,16 @@
     </row>
     <row r="51" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C51" s="1">
         <v>2020</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -2817,16 +2817,16 @@
     </row>
     <row r="52" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C52" s="1">
         <v>2020</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -2854,16 +2854,16 @@
     </row>
     <row r="53" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A53" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C53" s="1">
         <v>2024</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -2891,16 +2891,16 @@
     </row>
     <row r="54" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C54">
         <v>2019</v>
       </c>
       <c r="D54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -2928,16 +2928,16 @@
     </row>
     <row r="55" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C55" s="1">
         <v>2020</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -2965,16 +2965,16 @@
     </row>
     <row r="56" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C56" s="1">
         <v>2018</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
@@ -3002,16 +3002,16 @@
     </row>
     <row r="57" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -3039,16 +3039,16 @@
     </row>
     <row r="58" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C58" s="1">
         <v>2020</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -3076,16 +3076,16 @@
     </row>
     <row r="59" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A59" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C59" s="1">
         <v>2024</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -3113,16 +3113,16 @@
     </row>
     <row r="60" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C60" s="1">
         <v>2018</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -3150,16 +3150,16 @@
     </row>
     <row r="61" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C61" s="1">
         <v>2021</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
@@ -29587,40 +29587,39 @@
     <hyperlink ref="D30" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
     <hyperlink ref="D33" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
     <hyperlink ref="D37" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="D34" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="D36" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="D38" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="D35" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="D44" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="D43" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="D42" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="D40" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="D47" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="D45" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="D48" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="D51" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="D49" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="D52" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="D28" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="D57" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="D56" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="D55" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="D58" r:id="rId40" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="D60" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="D61" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="D17" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="D24" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="D4" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="D50" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="D22" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="D7" r:id="rId48" xr:uid="{AEC54F8E-3B97-0D42-BDBF-81F51CF558FA}"/>
-    <hyperlink ref="D10" r:id="rId49" xr:uid="{531FF59E-3ED0-7647-A071-9938F307CC65}"/>
-    <hyperlink ref="D32" r:id="rId50" xr:uid="{F44184D1-3BA6-CA4D-B592-38E9B7DD9585}"/>
-    <hyperlink ref="D41" r:id="rId51" xr:uid="{9B0CA447-45E8-D346-B56C-D40A5B7E7394}"/>
-    <hyperlink ref="D53" r:id="rId52" xr:uid="{6BBC2247-F5A6-2B4C-BCC0-65AE168D0F4C}"/>
-    <hyperlink ref="D59" r:id="rId53" xr:uid="{08F79F8D-E59F-AA49-A346-A986D8DD0952}"/>
-    <hyperlink ref="D13" r:id="rId54" xr:uid="{7C13DFA2-9F0D-4A4B-8033-EEC7EC90A886}"/>
-    <hyperlink ref="D39" r:id="rId55" xr:uid="{DC9C8D1E-F476-4A4E-902C-35F1A9CEBD2C}"/>
+    <hyperlink ref="D36" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="D38" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="D35" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D44" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="D43" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="D42" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="D40" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="D47" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="D45" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="D48" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="D51" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="D49" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="D52" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="D28" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="D57" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="D56" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="D55" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="D58" r:id="rId39" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="D60" r:id="rId40" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="D61" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="D17" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="D24" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="D4" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="D50" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="D22" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="D7" r:id="rId47" xr:uid="{AEC54F8E-3B97-0D42-BDBF-81F51CF558FA}"/>
+    <hyperlink ref="D10" r:id="rId48" xr:uid="{531FF59E-3ED0-7647-A071-9938F307CC65}"/>
+    <hyperlink ref="D32" r:id="rId49" xr:uid="{F44184D1-3BA6-CA4D-B592-38E9B7DD9585}"/>
+    <hyperlink ref="D41" r:id="rId50" xr:uid="{9B0CA447-45E8-D346-B56C-D40A5B7E7394}"/>
+    <hyperlink ref="D53" r:id="rId51" xr:uid="{6BBC2247-F5A6-2B4C-BCC0-65AE168D0F4C}"/>
+    <hyperlink ref="D59" r:id="rId52" xr:uid="{08F79F8D-E59F-AA49-A346-A986D8DD0952}"/>
+    <hyperlink ref="D13" r:id="rId53" xr:uid="{7C13DFA2-9F0D-4A4B-8033-EEC7EC90A886}"/>
+    <hyperlink ref="D39" r:id="rId54" xr:uid="{DC9C8D1E-F476-4A4E-902C-35F1A9CEBD2C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Uganda using 2023/2024 budget
</commit_message>
<xml_diff>
--- a/data/xlsx/metadata.xlsx
+++ b/data/xlsx/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/sites/codeforiati/gov-id-finder-data/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4F9421-27F2-1947-AB9F-0A1E97B3377A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80BD2DF-1AE3-CB49-869C-8554A73C6AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45200" yWindow="-2080" windowWidth="22260" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="186">
   <si>
     <t>Country_name</t>
   </si>
@@ -168,9 +168,6 @@
   </si>
   <si>
     <t>Uganda</t>
-  </si>
-  <si>
-    <t>https://datacatalog.worldbank.org/search/dataset/0038076</t>
   </si>
   <si>
     <t>https://drive.google.com/file/d/1joSpfyEyIk6IWnFxpn5Xhzhr1fuYhQv0/view?usp=sharing</t>
@@ -592,6 +589,9 @@
   <si>
     <t>https://assemblee-nationale.tg/wp-content/uploads/2023/12/LOI-de-FINANCES-2024-TAB.pdf</t>
   </si>
+  <si>
+    <t>https://budget.finance.go.ug/library/671</t>
+  </si>
 </sst>
 </file>
 
@@ -920,7 +920,7 @@
   <dimension ref="A1:AA1003"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -930,7 +930,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -967,7 +967,7 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>3</v>
@@ -976,7 +976,7 @@
         <v>2020</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1004,7 +1004,7 @@
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>4</v>
@@ -1041,16 +1041,16 @@
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C4" s="1">
         <v>2019</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -1078,7 +1078,7 @@
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>8</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>10</v>
@@ -1124,7 +1124,7 @@
         <v>2020</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1152,16 +1152,16 @@
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="1">
         <v>2019</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1189,10 +1189,10 @@
     </row>
     <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C8" s="1">
         <v>2014</v>
@@ -1226,10 +1226,10 @@
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C9" s="1">
         <v>2020</v>
@@ -1263,16 +1263,16 @@
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>156</v>
-      </c>
       <c r="C10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1300,10 +1300,10 @@
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C11" s="1">
         <v>2020</v>
@@ -1337,10 +1337,10 @@
     </row>
     <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C12" s="1">
         <v>2019</v>
@@ -1374,16 +1374,16 @@
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C13" s="1">
         <v>2024</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1411,10 +1411,10 @@
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C14" s="1">
         <v>2019</v>
@@ -1448,7 +1448,7 @@
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>11</v>
@@ -1485,10 +1485,10 @@
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C16" s="1">
         <v>2019</v>
@@ -1522,16 +1522,16 @@
     </row>
     <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C17" s="1">
         <v>2023</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1559,10 +1559,10 @@
     </row>
     <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C18" s="1">
         <v>2021</v>
@@ -1596,10 +1596,10 @@
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C19" s="1">
         <v>2017</v>
@@ -1633,16 +1633,16 @@
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C20" s="1">
         <v>2022</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1670,10 +1670,10 @@
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C21" s="1">
         <v>2015</v>
@@ -1707,16 +1707,16 @@
     </row>
     <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C22" s="1">
         <v>2020</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1744,16 +1744,16 @@
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C23">
         <v>2012</v>
       </c>
       <c r="D23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -1781,16 +1781,16 @@
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C24" s="1">
         <v>2018</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1818,10 +1818,10 @@
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C25" s="1">
         <v>2019</v>
@@ -1855,16 +1855,16 @@
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -1892,10 +1892,10 @@
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C27" s="1">
         <v>2020</v>
@@ -1929,10 +1929,10 @@
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C28" s="1">
         <v>2021</v>
@@ -1966,16 +1966,16 @@
     </row>
     <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C29">
         <v>2019</v>
       </c>
       <c r="D29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -2003,10 +2003,10 @@
     </row>
     <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C30" s="1">
         <v>2020</v>
@@ -2040,10 +2040,10 @@
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C31" s="1">
         <v>2021</v>
@@ -2077,16 +2077,16 @@
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C32" s="1">
         <v>2021</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2114,16 +2114,16 @@
     </row>
     <row r="33" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C33" s="1">
         <v>2020</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -2151,7 +2151,7 @@
     </row>
     <row r="34" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>25</v>
@@ -2160,7 +2160,7 @@
         <v>2024</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -2188,16 +2188,16 @@
     </row>
     <row r="35" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C35" s="1">
         <v>2017</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -2225,7 +2225,7 @@
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>26</v>
@@ -2262,10 +2262,10 @@
     </row>
     <row r="37" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C37" s="1">
         <v>2021</v>
@@ -2299,10 +2299,10 @@
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C38" s="1">
         <v>2020</v>
@@ -2336,16 +2336,16 @@
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C39" s="1">
         <v>2024</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -2373,16 +2373,16 @@
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C40" s="1">
         <v>2023</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -2410,16 +2410,16 @@
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C41" s="1">
         <v>2024</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -2447,10 +2447,10 @@
     </row>
     <row r="42" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C42" s="1">
         <v>2019</v>
@@ -2484,10 +2484,10 @@
     </row>
     <row r="43" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C43" s="1">
         <v>2021</v>
@@ -2521,7 +2521,7 @@
     </row>
     <row r="44" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>29</v>
@@ -2558,10 +2558,10 @@
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C45" s="1">
         <v>2021</v>
@@ -2595,16 +2595,16 @@
     </row>
     <row r="46" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C46">
         <v>2022</v>
       </c>
       <c r="D46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -2632,10 +2632,10 @@
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C47" s="1">
         <v>2019</v>
@@ -2669,16 +2669,16 @@
     </row>
     <row r="48" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -2706,7 +2706,7 @@
     </row>
     <row r="49" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>37</v>
@@ -2743,16 +2743,16 @@
     </row>
     <row r="50" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C50" s="1">
         <v>2022</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -2780,7 +2780,7 @@
     </row>
     <row r="51" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>35</v>
@@ -2817,10 +2817,10 @@
     </row>
     <row r="52" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C52" s="1">
         <v>2020</v>
@@ -2854,16 +2854,16 @@
     </row>
     <row r="53" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A53" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C53" s="1">
         <v>2024</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -2891,16 +2891,16 @@
     </row>
     <row r="54" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C54">
         <v>2023</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -2928,7 +2928,7 @@
     </row>
     <row r="55" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>43</v>
@@ -2937,7 +2937,7 @@
         <v>2024</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -2965,7 +2965,7 @@
     </row>
     <row r="56" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>41</v>
@@ -3002,16 +3002,16 @@
     </row>
     <row r="57" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -3039,16 +3039,16 @@
     </row>
     <row r="58" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C58" s="1">
-        <v>2020</v>
+      <c r="C58" s="1" t="s">
+        <v>153</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>45</v>
+      <c r="D58" s="4" t="s">
+        <v>185</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -3076,16 +3076,16 @@
     </row>
     <row r="59" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A59" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C59" s="1">
         <v>2024</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -3113,16 +3113,16 @@
     </row>
     <row r="60" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C60" s="1">
         <v>2018</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -3150,16 +3150,16 @@
     </row>
     <row r="61" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C61" s="1">
         <v>2021</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>

</xml_diff>

<commit_message>
Update Zambia from 2024 budget
</commit_message>
<xml_diff>
--- a/data/xlsx/metadata.xlsx
+++ b/data/xlsx/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/sites/codeforiati/gov-id-finder-data/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80BD2DF-1AE3-CB49-869C-8554A73C6AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21140575-24B4-E94B-A648-EBBEF81DBC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45200" yWindow="-2080" windowWidth="22260" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -168,9 +168,6 @@
   </si>
   <si>
     <t>Uganda</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1joSpfyEyIk6IWnFxpn5Xhzhr1fuYhQv0/view?usp=sharing</t>
   </si>
   <si>
     <t>Zimbabwe</t>
@@ -592,6 +589,9 @@
   <si>
     <t>https://budget.finance.go.ug/library/671</t>
   </si>
+  <si>
+    <t>https://www.mofnp.gov.zm/?page_id=4096</t>
+  </si>
 </sst>
 </file>
 
@@ -919,8 +919,8 @@
   </sheetPr>
   <dimension ref="A1:AA1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -930,7 +930,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -967,7 +967,7 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>3</v>
@@ -976,7 +976,7 @@
         <v>2020</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1004,7 +1004,7 @@
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>4</v>
@@ -1041,16 +1041,16 @@
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" s="1">
         <v>2019</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -1078,7 +1078,7 @@
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>8</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>10</v>
@@ -1124,7 +1124,7 @@
         <v>2020</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1152,16 +1152,16 @@
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" s="1">
         <v>2019</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1189,10 +1189,10 @@
     </row>
     <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C8" s="1">
         <v>2014</v>
@@ -1226,10 +1226,10 @@
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C9" s="1">
         <v>2020</v>
@@ -1263,16 +1263,16 @@
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>155</v>
-      </c>
       <c r="C10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1300,10 +1300,10 @@
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C11" s="1">
         <v>2020</v>
@@ -1337,10 +1337,10 @@
     </row>
     <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C12" s="1">
         <v>2019</v>
@@ -1374,16 +1374,16 @@
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C13" s="1">
         <v>2024</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1411,10 +1411,10 @@
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C14" s="1">
         <v>2019</v>
@@ -1448,7 +1448,7 @@
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>11</v>
@@ -1485,10 +1485,10 @@
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C16" s="1">
         <v>2019</v>
@@ -1522,16 +1522,16 @@
     </row>
     <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C17" s="1">
         <v>2023</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1559,10 +1559,10 @@
     </row>
     <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C18" s="1">
         <v>2021</v>
@@ -1596,10 +1596,10 @@
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C19" s="1">
         <v>2017</v>
@@ -1633,16 +1633,16 @@
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C20" s="1">
         <v>2022</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1670,10 +1670,10 @@
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C21" s="1">
         <v>2015</v>
@@ -1707,16 +1707,16 @@
     </row>
     <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C22" s="1">
         <v>2020</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1744,16 +1744,16 @@
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C23">
         <v>2012</v>
       </c>
       <c r="D23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -1781,16 +1781,16 @@
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C24" s="1">
         <v>2018</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1818,10 +1818,10 @@
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C25" s="1">
         <v>2019</v>
@@ -1855,16 +1855,16 @@
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -1892,10 +1892,10 @@
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C27" s="1">
         <v>2020</v>
@@ -1929,10 +1929,10 @@
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C28" s="1">
         <v>2021</v>
@@ -1966,16 +1966,16 @@
     </row>
     <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C29">
         <v>2019</v>
       </c>
       <c r="D29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -2003,10 +2003,10 @@
     </row>
     <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C30" s="1">
         <v>2020</v>
@@ -2040,10 +2040,10 @@
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C31" s="1">
         <v>2021</v>
@@ -2077,16 +2077,16 @@
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C32" s="1">
         <v>2021</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2114,16 +2114,16 @@
     </row>
     <row r="33" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C33" s="1">
         <v>2020</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -2151,7 +2151,7 @@
     </row>
     <row r="34" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>25</v>
@@ -2160,7 +2160,7 @@
         <v>2024</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -2188,16 +2188,16 @@
     </row>
     <row r="35" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C35" s="1">
         <v>2017</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -2225,7 +2225,7 @@
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>26</v>
@@ -2262,10 +2262,10 @@
     </row>
     <row r="37" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C37" s="1">
         <v>2021</v>
@@ -2299,10 +2299,10 @@
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C38" s="1">
         <v>2020</v>
@@ -2336,16 +2336,16 @@
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C39" s="1">
         <v>2024</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -2373,16 +2373,16 @@
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C40" s="1">
         <v>2023</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -2410,16 +2410,16 @@
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C41" s="1">
         <v>2024</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -2447,10 +2447,10 @@
     </row>
     <row r="42" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C42" s="1">
         <v>2019</v>
@@ -2484,10 +2484,10 @@
     </row>
     <row r="43" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C43" s="1">
         <v>2021</v>
@@ -2521,7 +2521,7 @@
     </row>
     <row r="44" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>29</v>
@@ -2558,10 +2558,10 @@
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C45" s="1">
         <v>2021</v>
@@ -2595,16 +2595,16 @@
     </row>
     <row r="46" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C46">
         <v>2022</v>
       </c>
       <c r="D46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -2632,10 +2632,10 @@
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C47" s="1">
         <v>2019</v>
@@ -2669,16 +2669,16 @@
     </row>
     <row r="48" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -2706,7 +2706,7 @@
     </row>
     <row r="49" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>37</v>
@@ -2743,16 +2743,16 @@
     </row>
     <row r="50" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C50" s="1">
         <v>2022</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -2780,7 +2780,7 @@
     </row>
     <row r="51" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>35</v>
@@ -2817,10 +2817,10 @@
     </row>
     <row r="52" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C52" s="1">
         <v>2020</v>
@@ -2854,16 +2854,16 @@
     </row>
     <row r="53" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A53" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C53" s="1">
         <v>2024</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -2891,16 +2891,16 @@
     </row>
     <row r="54" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C54">
         <v>2023</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -2928,7 +2928,7 @@
     </row>
     <row r="55" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>43</v>
@@ -2937,7 +2937,7 @@
         <v>2024</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -2965,7 +2965,7 @@
     </row>
     <row r="56" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>41</v>
@@ -3002,16 +3002,16 @@
     </row>
     <row r="57" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -3039,16 +3039,16 @@
     </row>
     <row r="58" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -3076,16 +3076,16 @@
     </row>
     <row r="59" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A59" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C59" s="1">
         <v>2024</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -3113,16 +3113,16 @@
     </row>
     <row r="60" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C60" s="1">
-        <v>2018</v>
+        <v>2024</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>45</v>
+      <c r="D60" s="4" t="s">
+        <v>185</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -3150,16 +3150,16 @@
     </row>
     <row r="61" spans="1:27" ht="42" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C61" s="1">
         <v>2021</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>

</xml_diff>

<commit_message>
Update Zimbabwe, NB new votes have been inserted; codelist appears to be sequential
</commit_message>
<xml_diff>
--- a/data/xlsx/metadata.xlsx
+++ b/data/xlsx/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/sites/codeforiati/gov-id-finder-data/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21140575-24B4-E94B-A648-EBBEF81DBC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E15F805-8ED7-1F42-9DE4-591C5AB44B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45200" yWindow="-2080" windowWidth="22260" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45180" yWindow="-2080" windowWidth="22260" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -171,9 +171,6 @@
   </si>
   <si>
     <t>Zimbabwe</t>
-  </si>
-  <si>
-    <t>https://www.cabri-sbo.org/uploads/bia/Zimbabwe_2021_Approval_External_EnactedBudget_MinFin_COMESASADC_English.pdf</t>
   </si>
   <si>
     <t>https://drive.google.com/file/d/1v9x2jU0apwlMu4F7PnDMfa1VPSLaTf9i/view?usp=sharing</t>
@@ -592,6 +589,9 @@
   <si>
     <t>https://www.mofnp.gov.zm/?page_id=4096</t>
   </si>
+  <si>
+    <t>https://www.zimtreasury.gov.zw/2024-budget-documents/?preview=true</t>
+  </si>
 </sst>
 </file>
 
@@ -919,8 +919,8 @@
   </sheetPr>
   <dimension ref="A1:AA1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -930,7 +930,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -967,7 +967,7 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>3</v>
@@ -976,7 +976,7 @@
         <v>2020</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1004,7 +1004,7 @@
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>4</v>
@@ -1041,16 +1041,16 @@
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C4" s="1">
         <v>2019</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -1078,7 +1078,7 @@
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>8</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>10</v>
@@ -1124,7 +1124,7 @@
         <v>2020</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1152,16 +1152,16 @@
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="1">
         <v>2019</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1189,10 +1189,10 @@
     </row>
     <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C8" s="1">
         <v>2014</v>
@@ -1226,10 +1226,10 @@
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C9" s="1">
         <v>2020</v>
@@ -1263,16 +1263,16 @@
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>154</v>
-      </c>
       <c r="C10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1300,10 +1300,10 @@
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C11" s="1">
         <v>2020</v>
@@ -1337,10 +1337,10 @@
     </row>
     <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C12" s="1">
         <v>2019</v>
@@ -1374,16 +1374,16 @@
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C13" s="1">
         <v>2024</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1411,10 +1411,10 @@
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C14" s="1">
         <v>2019</v>
@@ -1448,7 +1448,7 @@
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>11</v>
@@ -1485,10 +1485,10 @@
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C16" s="1">
         <v>2019</v>
@@ -1522,16 +1522,16 @@
     </row>
     <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C17" s="1">
         <v>2023</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1559,10 +1559,10 @@
     </row>
     <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C18" s="1">
         <v>2021</v>
@@ -1596,10 +1596,10 @@
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C19" s="1">
         <v>2017</v>
@@ -1633,16 +1633,16 @@
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C20" s="1">
         <v>2022</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1670,10 +1670,10 @@
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C21" s="1">
         <v>2015</v>
@@ -1707,16 +1707,16 @@
     </row>
     <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C22" s="1">
         <v>2020</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1744,16 +1744,16 @@
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C23">
         <v>2012</v>
       </c>
       <c r="D23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -1781,16 +1781,16 @@
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C24" s="1">
         <v>2018</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1818,10 +1818,10 @@
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C25" s="1">
         <v>2019</v>
@@ -1855,16 +1855,16 @@
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -1892,10 +1892,10 @@
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C27" s="1">
         <v>2020</v>
@@ -1929,10 +1929,10 @@
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C28" s="1">
         <v>2021</v>
@@ -1966,16 +1966,16 @@
     </row>
     <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C29">
         <v>2019</v>
       </c>
       <c r="D29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -2003,10 +2003,10 @@
     </row>
     <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C30" s="1">
         <v>2020</v>
@@ -2040,10 +2040,10 @@
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C31" s="1">
         <v>2021</v>
@@ -2077,16 +2077,16 @@
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C32" s="1">
         <v>2021</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2114,16 +2114,16 @@
     </row>
     <row r="33" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C33" s="1">
         <v>2020</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -2151,7 +2151,7 @@
     </row>
     <row r="34" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>25</v>
@@ -2160,7 +2160,7 @@
         <v>2024</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -2188,16 +2188,16 @@
     </row>
     <row r="35" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C35" s="1">
         <v>2017</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -2225,7 +2225,7 @@
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>26</v>
@@ -2262,10 +2262,10 @@
     </row>
     <row r="37" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C37" s="1">
         <v>2021</v>
@@ -2299,10 +2299,10 @@
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C38" s="1">
         <v>2020</v>
@@ -2336,16 +2336,16 @@
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C39" s="1">
         <v>2024</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -2373,16 +2373,16 @@
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C40" s="1">
         <v>2023</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -2410,16 +2410,16 @@
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C41" s="1">
         <v>2024</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -2447,10 +2447,10 @@
     </row>
     <row r="42" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C42" s="1">
         <v>2019</v>
@@ -2484,10 +2484,10 @@
     </row>
     <row r="43" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C43" s="1">
         <v>2021</v>
@@ -2521,7 +2521,7 @@
     </row>
     <row r="44" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>29</v>
@@ -2558,10 +2558,10 @@
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C45" s="1">
         <v>2021</v>
@@ -2595,16 +2595,16 @@
     </row>
     <row r="46" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C46">
         <v>2022</v>
       </c>
       <c r="D46" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -2632,10 +2632,10 @@
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C47" s="1">
         <v>2019</v>
@@ -2669,16 +2669,16 @@
     </row>
     <row r="48" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -2706,7 +2706,7 @@
     </row>
     <row r="49" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>37</v>
@@ -2743,16 +2743,16 @@
     </row>
     <row r="50" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C50" s="1">
         <v>2022</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -2780,7 +2780,7 @@
     </row>
     <row r="51" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>35</v>
@@ -2817,10 +2817,10 @@
     </row>
     <row r="52" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C52" s="1">
         <v>2020</v>
@@ -2854,16 +2854,16 @@
     </row>
     <row r="53" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A53" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C53" s="1">
         <v>2024</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -2891,16 +2891,16 @@
     </row>
     <row r="54" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C54">
         <v>2023</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -2928,7 +2928,7 @@
     </row>
     <row r="55" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>43</v>
@@ -2937,7 +2937,7 @@
         <v>2024</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -2965,7 +2965,7 @@
     </row>
     <row r="56" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>41</v>
@@ -3002,16 +3002,16 @@
     </row>
     <row r="57" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -3039,16 +3039,16 @@
     </row>
     <row r="58" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -3076,16 +3076,16 @@
     </row>
     <row r="59" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A59" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C59" s="1">
         <v>2024</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -3113,16 +3113,16 @@
     </row>
     <row r="60" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C60" s="1">
         <v>2024</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -3148,18 +3148,18 @@
       <c r="Z60" s="1"/>
       <c r="AA60" s="1"/>
     </row>
-    <row r="61" spans="1:27" ht="42" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C61" s="1">
-        <v>2021</v>
+        <v>2024</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>46</v>
+      <c r="D61" s="4" t="s">
+        <v>185</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>

</xml_diff>

<commit_message>
Update Côte d'Ivoire and Cameroon
</commit_message>
<xml_diff>
--- a/data/xlsx/metadata.xlsx
+++ b/data/xlsx/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/sites/codeforiati/gov-id-finder-data/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E15F805-8ED7-1F42-9DE4-591C5AB44B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3620625E-FF8C-FD41-A79A-3CEF61F6D231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45180" yWindow="-2080" windowWidth="22260" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44940" yWindow="-2080" windowWidth="22260" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,13 +71,7 @@
     <t>Cameroon</t>
   </si>
   <si>
-    <t>https://drive.google.com/file/d/1hgruayBV30fvEK1PrnMDhWbcfCT3T2HR/view?usp=sharing</t>
-  </si>
-  <si>
     <t>https://www.cabri-sbo.org/uploads/bia/CentralAfricanRepublic_2020_Approval_External_BudgetProposal_MinFin_CEN-SADECCAS_French_1.pdf</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1YR_DaQ-2eBAmXb63xPcxVS3lTStGq4tJ/view?usp=sharing</t>
   </si>
   <si>
     <t>https://www.cabri-sbo.org/uploads/bia/DemocraticRepublicofCongo_2021_Formulation_External_BudgetFramework_BudgetMin_COMESA_French.pdf</t>
@@ -90,9 +84,6 @@
   </si>
   <si>
     <t>https://www.cabri-sbo.org/uploads/bia/guinea_2017_approval_external_enacted_budget_ministry_of_finance_cen-sad_ecowas_french_.pdf</t>
-  </si>
-  <si>
-    <t>https://www.cabri-sbo.org/uploads/bia/guinea-bissau_2015_approval_external_enacted_budget_ministry_of_finance_cen-sad_ecowas_portuguese_.pdf</t>
   </si>
   <si>
     <t>https://drive.google.com/file/d/1PrJhGgHOfpJiKbcA1hapiqcQeNBny_AR/view?usp=sharing</t>
@@ -592,6 +583,15 @@
   <si>
     <t>https://www.zimtreasury.gov.zw/2024-budget-documents/?preview=true</t>
   </si>
+  <si>
+    <t>https://www.prc.cm/fr/multimedia/documents/9875-loi-n-2023-019-du-19-12-2023</t>
+  </si>
+  <si>
+    <t>https://www.dgbf.ci/wp-content/uploads/2024/01/Loi-de-Finances-Portant-Budget-de-lEtat-pour-lannee-2024.pdf</t>
+  </si>
+  <si>
+    <t>https://www.mef.gw/publicacoes/orcamento-geral-do-estado</t>
+  </si>
 </sst>
 </file>
 
@@ -919,8 +919,8 @@
   </sheetPr>
   <dimension ref="A1:AA1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -930,7 +930,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -967,7 +967,7 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>3</v>
@@ -976,7 +976,7 @@
         <v>2020</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1004,7 +1004,7 @@
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>4</v>
@@ -1041,16 +1041,16 @@
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C4" s="1">
         <v>2019</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -1078,7 +1078,7 @@
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>8</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>10</v>
@@ -1124,7 +1124,7 @@
         <v>2020</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1152,16 +1152,16 @@
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C7" s="1">
         <v>2019</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1189,10 +1189,10 @@
     </row>
     <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C8" s="1">
         <v>2014</v>
@@ -1226,10 +1226,10 @@
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C9" s="1">
         <v>2020</v>
@@ -1263,16 +1263,16 @@
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C10" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1300,16 +1300,16 @@
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C11" s="1">
         <v>2020</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1337,16 +1337,16 @@
     </row>
     <row r="12" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C12" s="1">
         <v>2019</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1374,16 +1374,16 @@
     </row>
     <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C13" s="1">
         <v>2024</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1411,16 +1411,16 @@
     </row>
     <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C14" s="1">
-        <v>2019</v>
+        <v>2024</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>14</v>
+      <c r="D14" s="4" t="s">
+        <v>184</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1448,16 +1448,16 @@
     </row>
     <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="1">
-        <v>2019</v>
+        <v>2024</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>12</v>
+      <c r="D15" s="4" t="s">
+        <v>183</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1485,16 +1485,16 @@
     </row>
     <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C16" s="1">
         <v>2019</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1522,16 +1522,16 @@
     </row>
     <row r="17" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C17" s="1">
         <v>2023</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1559,16 +1559,16 @@
     </row>
     <row r="18" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C18" s="1">
         <v>2021</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -1596,16 +1596,16 @@
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C19" s="1">
         <v>2017</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1633,16 +1633,16 @@
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C20" s="1">
         <v>2022</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1670,16 +1670,16 @@
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C21" s="1">
-        <v>2015</v>
+        <v>2024</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>19</v>
+      <c r="D21" s="4" t="s">
+        <v>185</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -1707,16 +1707,16 @@
     </row>
     <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C22" s="1">
         <v>2020</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1744,16 +1744,16 @@
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C23">
         <v>2012</v>
       </c>
       <c r="D23" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -1781,16 +1781,16 @@
     </row>
     <row r="24" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C24" s="1">
         <v>2018</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1818,16 +1818,16 @@
     </row>
     <row r="25" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C25" s="1">
         <v>2019</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -1855,16 +1855,16 @@
     </row>
     <row r="26" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -1892,16 +1892,16 @@
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C27" s="1">
         <v>2020</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -1929,16 +1929,16 @@
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C28" s="1">
         <v>2021</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -1966,16 +1966,16 @@
     </row>
     <row r="29" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C29">
         <v>2019</v>
       </c>
       <c r="D29" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -2003,16 +2003,16 @@
     </row>
     <row r="30" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C30" s="1">
         <v>2020</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -2040,16 +2040,16 @@
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C31" s="1">
         <v>2021</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -2077,16 +2077,16 @@
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C32" s="1">
         <v>2021</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -2114,16 +2114,16 @@
     </row>
     <row r="33" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C33" s="1">
         <v>2020</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -2151,16 +2151,16 @@
     </row>
     <row r="34" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C34" s="1">
         <v>2024</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -2188,16 +2188,16 @@
     </row>
     <row r="35" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C35" s="1">
         <v>2017</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -2225,16 +2225,16 @@
     </row>
     <row r="36" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C36" s="1">
         <v>2020</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -2262,16 +2262,16 @@
     </row>
     <row r="37" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C37" s="1">
         <v>2021</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -2299,16 +2299,16 @@
     </row>
     <row r="38" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C38" s="1">
         <v>2020</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2336,16 +2336,16 @@
     </row>
     <row r="39" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C39" s="1">
         <v>2024</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -2373,16 +2373,16 @@
     </row>
     <row r="40" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C40" s="1">
         <v>2023</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -2410,16 +2410,16 @@
     </row>
     <row r="41" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C41" s="1">
         <v>2024</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -2447,16 +2447,16 @@
     </row>
     <row r="42" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C42" s="1">
         <v>2019</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -2484,16 +2484,16 @@
     </row>
     <row r="43" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C43" s="1">
         <v>2021</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -2521,16 +2521,16 @@
     </row>
     <row r="44" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C44" s="1">
         <v>2021</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -2558,16 +2558,16 @@
     </row>
     <row r="45" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C45" s="1">
         <v>2021</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -2595,16 +2595,16 @@
     </row>
     <row r="46" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C46">
         <v>2022</v>
       </c>
       <c r="D46" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -2632,16 +2632,16 @@
     </row>
     <row r="47" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C47" s="1">
         <v>2019</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -2669,16 +2669,16 @@
     </row>
     <row r="48" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -2706,16 +2706,16 @@
     </row>
     <row r="49" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C49" s="1">
         <v>2020</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -2743,16 +2743,16 @@
     </row>
     <row r="50" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C50" s="1">
         <v>2022</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -2780,16 +2780,16 @@
     </row>
     <row r="51" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C51" s="1">
         <v>2020</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -2817,16 +2817,16 @@
     </row>
     <row r="52" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C52" s="1">
         <v>2020</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -2854,16 +2854,16 @@
     </row>
     <row r="53" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A53" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C53" s="1">
         <v>2024</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -2891,16 +2891,16 @@
     </row>
     <row r="54" spans="1:27" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C54">
         <v>2023</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -2926,18 +2926,18 @@
       <c r="Z54" s="1"/>
       <c r="AA54" s="1"/>
     </row>
-    <row r="55" spans="1:27" ht="14" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C55" s="1">
         <v>2024</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -2965,16 +2965,16 @@
     </row>
     <row r="56" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C56" s="1">
         <v>2018</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
@@ -3002,16 +3002,16 @@
     </row>
     <row r="57" spans="1:27" ht="28" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B57" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="D57" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -3039,16 +3039,16 @@
     </row>
     <row r="58" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -3076,16 +3076,16 @@
     </row>
     <row r="59" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A59" s="5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C59" s="1">
         <v>2024</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -3113,16 +3113,16 @@
     </row>
     <row r="60" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C60" s="1">
         <v>2024</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -3150,16 +3150,16 @@
     </row>
     <row r="61" spans="1:27" ht="14" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C61" s="1">
         <v>2024</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>

</xml_diff>